<commit_message>
Updated ICSD3-CFS and ICSD3-SOF mappings
</commit_message>
<xml_diff>
--- a/icsd3-mappings/icsd3-cfs-mapping.xlsx
+++ b/icsd3-mappings/icsd3-cfs-mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -270,12 +270,6 @@
     <t>ESS: Summary Score</t>
   </si>
   <si>
-    <t>ahi</t>
-  </si>
-  <si>
-    <t>Sleep Study: apnea hypopnea index</t>
-  </si>
-  <si>
     <t>&gt;10</t>
   </si>
   <si>
@@ -286,6 +280,84 @@
   </si>
   <si>
     <t>2,3,4</t>
+  </si>
+  <si>
+    <t>ahi3</t>
+  </si>
+  <si>
+    <t>Apnea / Hypopnea events with &gt;= 3% percent desaturation per hour of sleep</t>
+  </si>
+  <si>
+    <t>ahi_a0h3</t>
+  </si>
+  <si>
+    <t>AHI 3% -- all apneas and hypopneas with &gt;=3% oxygen desaturation</t>
+  </si>
+  <si>
+    <t>ahi_a0h3a</t>
+  </si>
+  <si>
+    <t>AHI 3% -- all apneas and hypopneas with &gt;=3% oxygen desaturation or arousal</t>
+  </si>
+  <si>
+    <t>ahi_a0h4</t>
+  </si>
+  <si>
+    <t>AHI 4% -- all apneas and hypopneas with &gt;=4% oxygen desaturation</t>
+  </si>
+  <si>
+    <t>ahi_a0h4a</t>
+  </si>
+  <si>
+    <t>AHI 4% -- all apneas and hypopneas with &gt;=4% oxygen desaturation or arousal</t>
+  </si>
+  <si>
+    <t>ahi_c0h3</t>
+  </si>
+  <si>
+    <t>Central AHI 3% -- central apneas and hypopneas with &gt;=3% oxygen desaturation</t>
+  </si>
+  <si>
+    <t>ahi_c0h3a</t>
+  </si>
+  <si>
+    <t>Central AHI 3% -- central apneas and hypopneas with &gt;=3% oxygen desaturation or arousal</t>
+  </si>
+  <si>
+    <t>ahi_c0h4</t>
+  </si>
+  <si>
+    <t>Central AHI 4% -- central apneas and hypopneas with &gt;=4% oxygen desaturation</t>
+  </si>
+  <si>
+    <t>ahi_c0h4a</t>
+  </si>
+  <si>
+    <t>Central AHI 4% -- central apneas and hypopneas with &gt;=4% oxygen desaturation or arousal</t>
+  </si>
+  <si>
+    <t>ahi_o0h3</t>
+  </si>
+  <si>
+    <t>Obstructive AHI 3% -- obstructive apneas and hypopneas with &gt;=3% oxygen desaturation</t>
+  </si>
+  <si>
+    <t>ahi_o0h3a</t>
+  </si>
+  <si>
+    <t>Obstructive AHI 3% -- obstructive apneas and hypopneas with &gt;=3% oxygen desaturation or arousal</t>
+  </si>
+  <si>
+    <t>ahi_o0h4</t>
+  </si>
+  <si>
+    <t>Obstructive AHI 4% -- obstructive apneas and hypopneas with &gt;=4% oxygen desaturation</t>
+  </si>
+  <si>
+    <t>ahi_o0h4a</t>
+  </si>
+  <si>
+    <t>Obstructive AHI 4% -- obstructive apneas and hypopneas with &gt;=4% oxygen desaturation or arousal</t>
   </si>
 </sst>
 </file>
@@ -623,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD75"/>
+      <selection activeCell="A54" sqref="A54:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -663,7 +735,7 @@
         <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -691,7 +763,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -705,7 +777,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -719,7 +791,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -733,7 +805,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -747,7 +819,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -761,7 +833,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -789,7 +861,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -803,7 +875,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -817,7 +889,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1189,21 +1261,285 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" t="s">
-        <v>85</v>
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>